<commit_message>
Added handling of common namespaces.
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361A1A5E-40D2-4678-970D-1CE4E4DE683B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E75E7F8-F806-4026-B305-7DDEF68A74A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -235,6 +235,22 @@
   </si>
   <si>
     <t>Remove sequences or flowcharts that are empty or contain only one activity.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented Comment Out activity</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UndocumentedCommentOut.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Workflows should only have the necessary activities for its execution, and activities that are commented out or that are not connected to any node in a flowchart should be removed. If there is need to keep commented activities, add annotations to describe the reason.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Consider removing unreachable activities.</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -453,6 +469,10 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$12" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$2" lockText="1" noThreeD="1"/>
 </file>
 
@@ -1117,6 +1137,73 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>234950</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>273050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>438150</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>514350</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1044"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9C6BA62-E39E-4BE0-AAA5-B1072F934391}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1498,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1721,6 +1808,24 @@
         <v>53</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="A12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1944,6 +2049,28 @@
                     <xdr:colOff>400050</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>1327150</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1044" r:id="rId14" name="Check Box 20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>234950</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>273050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>438150</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>514350</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
Implemented Unreachable Activities test.
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E75E7F8-F806-4026-B305-7DDEF68A74A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5FB24A-6AC6-49D0-AAD5-1B695CE1C9CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -238,19 +238,19 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Undocumented Comment Out activity</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UndocumentedCommentOut.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Workflows should only have the necessary activities for its execution, and activities that are commented out or that are not connected to any node in a flowchart should be removed. If there is need to keep commented activities, add annotations to describe the reason.</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Consider removing unreachable activities.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Unreachable activities</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UnreachableActivities.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -392,7 +392,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -424,9 +424,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,7 +441,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,13 +514,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>209550</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>488950</xdr:rowOff>
+          <xdr:rowOff>485775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>730250</xdr:rowOff>
+          <xdr:rowOff>733425</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -584,13 +581,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>387350</xdr:rowOff>
+          <xdr:rowOff>390525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>400050</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>635000</xdr:rowOff>
+          <xdr:rowOff>638175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -649,15 +646,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>215900</xdr:colOff>
+          <xdr:colOff>219075</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>508000</xdr:rowOff>
+          <xdr:rowOff>504825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>749300</xdr:rowOff>
+          <xdr:rowOff>752475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -716,7 +713,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>254000</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>685800</xdr:rowOff>
         </xdr:from>
@@ -724,7 +721,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>927100</xdr:rowOff>
+          <xdr:rowOff>923925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -783,13 +780,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>222250</xdr:colOff>
+          <xdr:colOff>219075</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>749300</xdr:rowOff>
+          <xdr:rowOff>752475</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>425450</xdr:colOff>
+          <xdr:colOff>428625</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>990600</xdr:rowOff>
         </xdr:to>
@@ -850,13 +847,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>260350</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>806450</xdr:rowOff>
+          <xdr:rowOff>809625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>463550</xdr:colOff>
+          <xdr:colOff>466725</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>1047750</xdr:rowOff>
         </xdr:to>
@@ -923,9 +920,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>450850</xdr:colOff>
+          <xdr:colOff>447675</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>850900</xdr:rowOff>
+          <xdr:rowOff>847725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -990,9 +987,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>450850</xdr:colOff>
+          <xdr:colOff>447675</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>812800</xdr:rowOff>
+          <xdr:rowOff>809625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1051,7 +1048,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>254000</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>895350</xdr:rowOff>
         </xdr:from>
@@ -1059,7 +1056,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>457200</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>1136650</xdr:rowOff>
+          <xdr:rowOff>1133475</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1118,7 +1115,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>196850</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>1085850</xdr:rowOff>
         </xdr:from>
@@ -1126,7 +1123,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>400050</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>1327150</xdr:rowOff>
+          <xdr:rowOff>1323975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1185,9 +1182,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>234950</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>273050</xdr:rowOff>
+          <xdr:rowOff>276225</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
@@ -1203,7 +1200,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9C6BA62-E39E-4BE0-AAA5-B1072F934391}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1259,11 +1256,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>444500</xdr:rowOff>
+          <xdr:rowOff>447675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>431800</xdr:colOff>
+          <xdr:colOff>428625</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>685800</xdr:rowOff>
         </xdr:to>
@@ -1591,15 +1588,15 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="11"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.4140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.9140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="39.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.625" style="1"/>
+    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1622,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="90">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="10" t="b">
         <v>1</v>
       </c>
@@ -1640,7 +1637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="72">
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="75">
       <c r="A3" s="10" t="b">
         <v>1</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="90">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="10" t="b">
         <v>1</v>
       </c>
@@ -1676,8 +1673,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="126">
-      <c r="A5" s="12" t="b">
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="131.25">
+      <c r="A5" s="11" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1694,8 +1691,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="144">
-      <c r="A6" s="12" t="b">
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="150">
+      <c r="A6" s="11" t="b">
         <v>0</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1714,7 +1711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="144">
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="150">
       <c r="A7" s="10" t="b">
         <v>0</v>
       </c>
@@ -1734,7 +1731,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="108">
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="112.5">
       <c r="A8" s="10" t="b">
         <v>1</v>
       </c>
@@ -1752,7 +1749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="108">
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="112.5">
       <c r="A9" s="10" t="b">
         <v>1</v>
       </c>
@@ -1770,7 +1767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" ht="162">
+    <row r="10" spans="1:6" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="10" t="b">
         <v>1</v>
       </c>
@@ -1790,8 +1787,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="180">
-      <c r="A11" s="16" t="b">
+    <row r="11" spans="1:6" ht="187.5">
+      <c r="A11" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1808,22 +1805,22 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="90">
-      <c r="A12" s="16" t="b">
+    <row r="12" spans="1:6" ht="93.75">
+      <c r="A12" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1844,13 +1841,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>209550</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>488950</xdr:rowOff>
+                    <xdr:rowOff>485775</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>730250</xdr:rowOff>
+                    <xdr:rowOff>733425</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1866,13 +1863,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>387350</xdr:rowOff>
+                    <xdr:rowOff>390525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>400050</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>635000</xdr:rowOff>
+                    <xdr:rowOff>638175</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1886,15 +1883,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>215900</xdr:colOff>
+                    <xdr:colOff>219075</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>508000</xdr:rowOff>
+                    <xdr:rowOff>504825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>749300</xdr:rowOff>
+                    <xdr:rowOff>752475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1908,7 +1905,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>254000</xdr:colOff>
+                    <xdr:colOff>257175</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>685800</xdr:rowOff>
                   </from>
@@ -1916,7 +1913,7 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>927100</xdr:rowOff>
+                    <xdr:rowOff>923925</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1930,13 +1927,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>222250</xdr:colOff>
+                    <xdr:colOff>219075</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>749300</xdr:rowOff>
+                    <xdr:rowOff>752475</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>425450</xdr:colOff>
+                    <xdr:colOff>428625</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>990600</xdr:rowOff>
                   </to>
@@ -1952,13 +1949,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>260350</xdr:colOff>
+                    <xdr:colOff>257175</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>806450</xdr:rowOff>
+                    <xdr:rowOff>809625</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>463550</xdr:colOff>
+                    <xdr:colOff>466725</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>1047750</xdr:rowOff>
                   </to>
@@ -1980,9 +1977,9 @@
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>450850</xdr:colOff>
+                    <xdr:colOff>447675</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>850900</xdr:rowOff>
+                    <xdr:rowOff>847725</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2002,9 +1999,9 @@
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>450850</xdr:colOff>
+                    <xdr:colOff>447675</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>812800</xdr:rowOff>
+                    <xdr:rowOff>809625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2018,7 +2015,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>254000</xdr:colOff>
+                    <xdr:colOff>257175</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>895350</xdr:rowOff>
                   </from>
@@ -2026,7 +2023,7 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>457200</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>1136650</xdr:rowOff>
+                    <xdr:rowOff>1133475</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2040,7 +2037,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>196850</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>1085850</xdr:rowOff>
                   </from>
@@ -2048,7 +2045,7 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>400050</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>1327150</xdr:rowOff>
+                    <xdr:rowOff>1323975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2062,9 +2059,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>234950</xdr:colOff>
+                    <xdr:colOff>238125</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>273050</xdr:rowOff>
+                    <xdr:rowOff>276225</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
@@ -2091,21 +2088,21 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.4140625" customWidth="1"/>
-    <col min="5" max="5" width="49.83203125" customWidth="1"/>
-    <col min="6" max="6" width="40.08203125" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="49.875" customWidth="1"/>
+    <col min="6" max="6" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -2121,11 +2118,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="90">
-      <c r="A2" s="13" t="b">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="93.75">
+      <c r="A2" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2157,11 +2154,11 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>444500</xdr:rowOff>
+                    <xdr:rowOff>447675</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>431800</xdr:colOff>
+                    <xdr:colOff>428625</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>685800</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
Modularized checks, created Severity check column and changed SimulateClick and SimulateType checks to also look for SendWindowMessages.
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5FB24A-6AC6-49D0-AAD5-1B695CE1C9CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB233C6-C71F-4562-9E1D-BA3EFC248F48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -147,38 +147,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>SimulateClick not used</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UseSimulateClick.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Since it does not depend on the mouse driver, SimulateClick provides a faster and more robust way to perform clicks, so it should be used whenever possible. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateClick if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>SimulateType not used</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UseSimulateType.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Since it does not depend on the keyboard driver, SimulateType provides a faster and more robust way to perform type actions, so it should be used whenever possible. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateType if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>The idx attribute is used to distinguish elements with the same selector based on their order in the interface hierarchy. This order can change if the elements on the screen change, so the value for the idx attribute should be kept to a low value to avoid the selection of wrong elements. This checks receives a threshold for the value of the idx attribute. For more about selectors, refer to https://studio.uipath.com/docs/ui-automation#section-selectors</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -246,11 +214,67 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Unreachable activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UnreachableActivities.xaml</t>
+    <t>Severity</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Low</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Severity</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Low</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Checks\UndocumentedDefaultClick.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Use SimulateClick or SendWindowMessages if the target control supports it.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Since they do not depend on the mouse driver, the properties SimulateClick and SendWindowMessages provide a faster and more robust way to perform clicks, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Since they do not depend on the keyboard driver, the properties SimulateType and SendWindowMessages provide a faster and more robust way to perform typing actions, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Use SimulateType or SendWindowMessages if the target control supports it.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UndocumentedDefaultType.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented default type</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented default click</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented unreachable activities</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -1582,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -1593,15 +1617,15 @@
     <col min="1" max="1" width="8.625" style="1"/>
     <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="39.625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.625" style="1"/>
+    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>4</v>
@@ -1612,14 +1636,17 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="10" t="b">
         <v>1</v>
       </c>
@@ -1630,14 +1657,17 @@
         <v>7</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="75">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="10" t="b">
         <v>1</v>
       </c>
@@ -1648,14 +1678,17 @@
         <v>9</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="93.75">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="10" t="b">
         <v>1</v>
       </c>
@@ -1666,14 +1699,17 @@
         <v>16</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="131.25">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="11" t="b">
         <v>1</v>
       </c>
@@ -1684,14 +1720,17 @@
         <v>18</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="150">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="11" t="b">
         <v>0</v>
       </c>
@@ -1704,14 +1743,17 @@
       <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="150">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="10" t="b">
         <v>0</v>
       </c>
@@ -1724,103 +1766,121 @@
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="112.5">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="4" t="s">
-        <v>33</v>
+      <c r="E8" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>34</v>
+        <v>56</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="112.5">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="4" t="s">
-        <v>37</v>
+      <c r="E9" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>38</v>
+        <v>57</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" ht="168.75">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>39</v>
+      <c r="E10" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="187.5">
+    <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="4" t="s">
-        <v>50</v>
+      <c r="E11" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="93.75">
+    <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="4" t="s">
-        <v>54</v>
+      <c r="E12" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2082,10 +2142,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2093,17 +2153,17 @@
     <col min="1" max="1" width="8.625" customWidth="1"/>
     <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="4" width="28.375" customWidth="1"/>
-    <col min="5" max="5" width="49.875" customWidth="1"/>
-    <col min="6" max="6" width="40.125" customWidth="1"/>
+    <col min="4" max="5" width="28.375" customWidth="1"/>
+    <col min="6" max="6" width="49.875" customWidth="1"/>
+    <col min="7" max="7" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -2111,29 +2171,35 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="12" t="b">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
-        <v>43</v>
+      <c r="E2" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rephrasing suggestion of EmptyCatch check.
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB233C6-C71F-4562-9E1D-BA3EFC248F48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB36F96-3D1D-4C1F-B8E9-84011C1940EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,10 +103,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>If no action is taken to handle the exception, include at least a Log Message activity and Rethrow it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Variables not following naming convention</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -275,6 +271,10 @@
   </si>
   <si>
     <t>Checks\UndocumentedUnreachableActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>If no action is taken to handle the exception, consider including at least a Log Message activity and Rethrow it.</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -1625,7 +1625,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>4</v>
@@ -1637,7 +1637,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>15</v>
@@ -1721,13 +1721,13 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1735,22 +1735,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1758,22 +1758,22 @@
         <v>0</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1781,20 +1781,20 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1802,20 +1802,20 @@
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
@@ -1823,22 +1823,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187.5">
@@ -1846,20 +1846,20 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="93.75">
@@ -1867,20 +1867,20 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2160,10 +2160,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -2172,7 +2172,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -2186,20 +2186,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>